<commit_message>
Modified ProductList and Excel file
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="92">
   <si>
     <t xml:space="preserve">SIRA</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Model</t>
   </si>
   <si>
+    <t xml:space="preserve">Link</t>
+  </si>
+  <si>
     <t xml:space="preserve">BT-ANV-00-000-HLD-P3B2-01</t>
   </si>
   <si>
@@ -80,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">İlk ürün</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/btk42/BT-ANV-00-000-HLD-P3B2-01</t>
   </si>
   <si>
     <t xml:space="preserve">BT-ANV-00-000-SLD-H3B0-01</t>
@@ -495,10 +501,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -542,40 +548,46 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,34 +595,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -618,34 +630,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,34 +665,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,34 +700,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,34 +735,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,34 +770,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,34 +805,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="K9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,34 +840,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -863,34 +875,34 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -898,34 +910,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,34 +945,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,34 +980,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,34 +1015,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,34 +1050,34 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,34 +1085,34 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1108,34 +1120,34 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,34 +1155,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,34 +1190,34 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,34 +1225,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1248,34 +1260,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1283,34 +1295,34 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,34 +1330,34 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,34 +1365,34 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="J25" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,34 +1400,34 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1423,34 +1435,34 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1458,34 +1470,34 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,34 +1505,34 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1528,34 +1540,34 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,34 +1575,34 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,34 +1610,34 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,34 +1645,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1668,34 +1680,34 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="G34" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,34 +1715,34 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,34 +1750,34 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,34 +1785,34 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,34 +1820,34 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1843,34 +1855,34 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"BT-ANV-00-000-HLD-P3B1-01" PCB'si için excel'e link eklendi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="89">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -288,13 +288,16 @@
   </si>
   <si>
     <t>Sıra</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-ANV-00-000-HLD-P3B1-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -324,6 +327,14 @@
       <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="2">
@@ -358,10 +369,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -390,8 +402,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -740,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -825,7 +841,9 @@
       <c r="J2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="9"/>
+      <c r="K2" s="10" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
@@ -2097,8 +2115,11 @@
       <c r="J43" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Butonlar klasörüne Bombeli Button projesi eklendi. (BT-BOM-OS-000-SLD-P2B1-03)
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EARGE8PC\Desktop\btk42GithubIo\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18375C5B-4FB8-4DEF-B23B-D95ED75ABFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="93">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -291,12 +292,24 @@
   </si>
   <si>
     <t>https://github.com/btk42/BT-ANV-00-000-HLD-P3B1-01</t>
+  </si>
+  <si>
+    <t>BT-BOM-OS-000-SLD-P2B1-03</t>
+  </si>
+  <si>
+    <t>Bombeli</t>
+  </si>
+  <si>
+    <t>Model-03</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/Bombeli_Button_One-Shot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -373,30 +386,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -404,6 +408,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -753,11 +760,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -771,1355 +778,1340 @@
     <col min="8" max="8" width="15.88671875" style="1" customWidth="1"/>
     <col min="9" max="9" width="18.88671875" style="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" customWidth="1"/>
-    <col min="11" max="11" width="47.44140625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="2"/>
+    <col min="11" max="11" width="47.44140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" s="10" t="s">
+      <c r="J2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="9"/>
+      <c r="I3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" s="9"/>
+      <c r="I4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K5" s="9"/>
+      <c r="J5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K6" s="9"/>
+      <c r="I6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K7" s="9"/>
+      <c r="J7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K8" s="9"/>
+      <c r="I8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K9" s="9"/>
+      <c r="J9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="9"/>
+      <c r="I10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" s="9"/>
+      <c r="J11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="D12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="9"/>
+      <c r="J12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="9"/>
+      <c r="J13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K14" s="9"/>
+      <c r="J14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="D15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K15" s="9"/>
+      <c r="I15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="D16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="9"/>
+      <c r="I16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="D17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K17" s="9"/>
+      <c r="I17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="D18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K18" s="9"/>
+      <c r="I18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="8" t="s">
+      <c r="D19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="9"/>
+      <c r="I19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="D20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K20" s="9"/>
+      <c r="I20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="8" t="s">
+      <c r="D21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K21" s="9"/>
+      <c r="I21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="8" t="s">
+      <c r="D22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K22" s="9"/>
+      <c r="I22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K23" s="9"/>
+      <c r="I23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="D24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I24" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K24" s="9"/>
+      <c r="I24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="8" t="s">
+      <c r="D25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K25" s="9"/>
+      <c r="I25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="8" t="s">
+      <c r="D26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K26" s="9"/>
+      <c r="I26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K27" s="9"/>
+      <c r="J27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K28" s="9"/>
+      <c r="J28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="D29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J29" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K29" s="9"/>
+      <c r="J29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="8" t="s">
+      <c r="C30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K30" s="9"/>
+      <c r="I30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="8" t="s">
+      <c r="D31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K31" s="9"/>
+      <c r="I31" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="8" t="s">
+      <c r="D32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K32" s="9"/>
+      <c r="I32" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K32" s="6"/>
     </row>
     <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="8" t="s">
+      <c r="D33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I33" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K33" s="9"/>
+      <c r="I33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K33" s="6"/>
     </row>
     <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="8" t="s">
+      <c r="D34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I34" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K34" s="9"/>
+      <c r="I34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K34" s="6"/>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="8" t="s">
+      <c r="D35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K35" s="9"/>
+      <c r="I35" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K35" s="6"/>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="8" t="s">
+      <c r="D36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K36" s="9"/>
+      <c r="I36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K36" s="6"/>
     </row>
     <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
+      <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="8" t="s">
+      <c r="D37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="H37" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I37" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K37" s="9"/>
+      <c r="I37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K37" s="6"/>
     </row>
     <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
+      <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="8" t="s">
+      <c r="D38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H38" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I38" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K38" s="9"/>
+      <c r="I38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K38" s="6"/>
     </row>
     <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
+      <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="8" t="s">
+      <c r="D39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G39" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="H39" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K39" s="9"/>
-    </row>
-    <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="I39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K39" s="6"/>
+    </row>
+    <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K40" r:id="rId2" xr:uid="{0C4CECC9-1CEB-446B-8CC9-551B0A48D379}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Buton sıra numarası güncellendi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18375C5B-4FB8-4DEF-B23B-D95ED75ABFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDBBF96-5FF1-490E-9476-364639AF0348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,7 +358,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -381,12 +381,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -411,6 +422,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -763,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2074,6 +2088,9 @@
       <c r="K39" s="6"/>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="9">
+        <v>39</v>
+      </c>
       <c r="B40" s="5" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
BT-B18-OS-000-HLD-P3B1-01 için URL eklendi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDBBF96-5FF1-490E-9476-364639AF0348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D721BF-8224-43F5-8EC4-144D88381408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="94">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/Bombeli_Button_One-Shot</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/Button_One_Shot</t>
   </si>
 </sst>
 </file>
@@ -777,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1263,9 @@
       <c r="J14" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">

</xml_diff>

<commit_message>
Bombeli Buton ve Buton Akbil URL uzantıları güncellendi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D721BF-8224-43F5-8EC4-144D88381408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4EBB6A-CAA8-4FD9-B2B0-A95DEE231031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -303,10 +303,10 @@
     <t>Model-03</t>
   </si>
   <si>
-    <t>https://github.com/btk42/Bombeli_Button_One-Shot</t>
-  </si>
-  <si>
     <t>https://github.com/btk42/Button_One_Shot</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-BOM-OS-000-SLD-P2B1-03</t>
   </si>
 </sst>
 </file>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1264,7 @@
         <v>84</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2124,7 +2124,7 @@
         <v>91</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Capacitive Buton URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4EBB6A-CAA8-4FD9-B2B0-A95DEE231031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53326B3D-3EC3-48C5-B8BB-BCA77FA0FAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="95">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/BT-BOM-OS-000-SLD-P2B1-03</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-B18-00-TCH-SLD-P2B0-01</t>
   </si>
 </sst>
 </file>
@@ -780,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -795,7 +798,7 @@
     <col min="8" max="8" width="15.88671875" style="1" customWidth="1"/>
     <col min="9" max="9" width="18.88671875" style="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" customWidth="1"/>
-    <col min="11" max="11" width="47.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="49.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
@@ -2090,7 +2093,9 @@
       <c r="J39" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="K39" s="6"/>
+      <c r="K39" s="7" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
@@ -2131,9 +2136,10 @@
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="K40" r:id="rId2" xr:uid="{0C4CECC9-1CEB-446B-8CC9-551B0A48D379}"/>
+    <hyperlink ref="K39" r:id="rId3" xr:uid="{6EB826D2-EB5D-44F7-87F6-6175AD30B3AB}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Capacitive butonun kodu değiştirildi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53326B3D-3EC3-48C5-B8BB-BCA77FA0FAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8918D82-31E0-4A37-844F-5D1F394D92DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -264,9 +264,6 @@
     <t>BT-PRL-00-MSC-DLD-S2B0-01</t>
   </si>
   <si>
-    <t>BT-B18-00-TCH-SLD-P2B0-01</t>
-  </si>
-  <si>
     <t>Touch Buton</t>
   </si>
   <si>
@@ -309,7 +306,10 @@
     <t>https://github.com/btk42/BT-BOM-OS-000-SLD-P2B1-03</t>
   </si>
   <si>
-    <t>https://github.com/btk42/BT-B18-00-TCH-SLD-P2B0-01</t>
+    <t>BT-B18-OS-TCH-HLD-P3B2-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-B18-OS-TCH-HLD-P3B2-01</t>
   </si>
 </sst>
 </file>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -804,7 +804,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -842,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
@@ -866,10 +866,10 @@
         <v>29</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -901,7 +901,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K3" s="6"/>
     </row>
@@ -934,7 +934,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K4" s="6"/>
     </row>
@@ -943,7 +943,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -967,7 +967,7 @@
         <v>29</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K5" s="6"/>
     </row>
@@ -1000,7 +1000,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -1033,7 +1033,7 @@
         <v>29</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -1066,7 +1066,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -1099,7 +1099,7 @@
         <v>29</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K9" s="6"/>
     </row>
@@ -1132,7 +1132,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K10" s="6"/>
     </row>
@@ -1141,7 +1141,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>34</v>
@@ -1165,7 +1165,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K11" s="6"/>
     </row>
@@ -1198,7 +1198,7 @@
         <v>29</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K12" s="6"/>
     </row>
@@ -1231,7 +1231,7 @@
         <v>29</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K13" s="6"/>
     </row>
@@ -1264,10 +1264,10 @@
         <v>29</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1299,7 +1299,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K15" s="6"/>
     </row>
@@ -1332,7 +1332,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K16" s="6"/>
     </row>
@@ -1365,7 +1365,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K17" s="6"/>
     </row>
@@ -1398,7 +1398,7 @@
         <v>19</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K18" s="6"/>
     </row>
@@ -1431,7 +1431,7 @@
         <v>19</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K19" s="6"/>
     </row>
@@ -1464,7 +1464,7 @@
         <v>19</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K20" s="6"/>
     </row>
@@ -1497,7 +1497,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K21" s="6"/>
     </row>
@@ -1530,7 +1530,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -1563,7 +1563,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K23" s="6"/>
     </row>
@@ -1581,7 +1581,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>17</v>
@@ -1596,7 +1596,7 @@
         <v>19</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K24" s="6"/>
     </row>
@@ -1629,7 +1629,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K25" s="6"/>
     </row>
@@ -1662,7 +1662,7 @@
         <v>19</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K26" s="6"/>
     </row>
@@ -1695,7 +1695,7 @@
         <v>15</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K27" s="6"/>
     </row>
@@ -1728,7 +1728,7 @@
         <v>15</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K28" s="6"/>
     </row>
@@ -1761,7 +1761,7 @@
         <v>15</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K29" s="6"/>
     </row>
@@ -1770,7 +1770,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>11</v>
@@ -1779,7 +1779,7 @@
         <v>11</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>21</v>
@@ -1794,7 +1794,7 @@
         <v>19</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K30" s="6"/>
     </row>
@@ -1827,7 +1827,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K31" s="6"/>
     </row>
@@ -1860,7 +1860,7 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K32" s="6"/>
     </row>
@@ -1893,7 +1893,7 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K33" s="6"/>
     </row>
@@ -1926,7 +1926,7 @@
         <v>19</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K34" s="6"/>
     </row>
@@ -1959,7 +1959,7 @@
         <v>19</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K35" s="6"/>
     </row>
@@ -1992,7 +1992,7 @@
         <v>19</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K36" s="6"/>
     </row>
@@ -2025,7 +2025,7 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K37" s="6"/>
     </row>
@@ -2058,7 +2058,7 @@
         <v>19</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K38" s="6"/>
     </row>
@@ -2067,31 +2067,31 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K39" s="7" t="s">
         <v>94</v>
@@ -2102,10 +2102,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>25</v>
@@ -2126,10 +2126,10 @@
         <v>29</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Button Fan için URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8918D82-31E0-4A37-844F-5D1F394D92DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D9E03B-976D-4491-A169-BD3993547E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="96">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/BT-B18-OS-TCH-HLD-P3B2-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-B18-00-FAN-SLD-P1B0-01</t>
   </si>
 </sst>
 </file>
@@ -783,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1664,7 +1667,9 @@
       <c r="J26" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K26" s="6"/>
+      <c r="K26" s="7" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
@@ -2137,9 +2142,10 @@
     <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="K40" r:id="rId2" xr:uid="{0C4CECC9-1CEB-446B-8CC9-551B0A48D379}"/>
     <hyperlink ref="K39" r:id="rId3" xr:uid="{6EB826D2-EB5D-44F7-87F6-6175AD30B3AB}"/>
+    <hyperlink ref="K26" r:id="rId4" xr:uid="{8C79113F-7200-4455-9613-1DB76805CFBD}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Button 18 one shot için URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D9E03B-976D-4491-A169-BD3993547E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106679D6-DEC3-419E-AC28-62765F32245E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -300,9 +300,6 @@
     <t>Model-03</t>
   </si>
   <si>
-    <t>https://github.com/btk42/Button_One_Shot</t>
-  </si>
-  <si>
     <t>https://github.com/btk42/BT-BOM-OS-000-SLD-P2B1-03</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/BT-B18-00-FAN-SLD-P1B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-B18-OS-000-HLD-P3B1-01</t>
   </si>
 </sst>
 </file>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1269,8 +1269,8 @@
       <c r="J14" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K14" s="6" t="s">
-        <v>91</v>
+      <c r="K14" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1668,7 +1668,7 @@
         <v>83</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2072,7 +2072,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>36</v>
@@ -2099,7 +2099,7 @@
         <v>83</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2134,7 +2134,7 @@
         <v>90</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2143,9 +2143,10 @@
     <hyperlink ref="K40" r:id="rId2" xr:uid="{0C4CECC9-1CEB-446B-8CC9-551B0A48D379}"/>
     <hyperlink ref="K39" r:id="rId3" xr:uid="{6EB826D2-EB5D-44F7-87F6-6175AD30B3AB}"/>
     <hyperlink ref="K26" r:id="rId4" xr:uid="{8C79113F-7200-4455-9613-1DB76805CFBD}"/>
+    <hyperlink ref="K14" r:id="rId5" xr:uid="{F83E4073-CF8D-4CCE-A9AD-3FC7038B5513}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Eka 7 li buton URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106679D6-DEC3-419E-AC28-62765F32245E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FC1497-0BCD-4F2A-82AB-E7EB8C53F885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="97">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/BT-B18-OS-000-HLD-P3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-EKA-00-7BT-DLD-S2B0-01</t>
   </si>
 </sst>
 </file>
@@ -786,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1966,7 +1969,9 @@
       <c r="J35" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K35" s="6"/>
+      <c r="K35" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
@@ -2144,9 +2149,10 @@
     <hyperlink ref="K39" r:id="rId3" xr:uid="{6EB826D2-EB5D-44F7-87F6-6175AD30B3AB}"/>
     <hyperlink ref="K26" r:id="rId4" xr:uid="{8C79113F-7200-4455-9613-1DB76805CFBD}"/>
     <hyperlink ref="K14" r:id="rId5" xr:uid="{F83E4073-CF8D-4CCE-A9AD-3FC7038B5513}"/>
+    <hyperlink ref="K35" r:id="rId6" xr:uid="{4DFC5FA9-97DC-48EE-B349-9B499628461D}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Antivandal Butonların Alt Grup Özellikleri Güncellendi
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BTK\Ürün_Listesi\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FC1497-0BCD-4F2A-82AB-E7EB8C53F885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AC1311-57DF-4291-BE02-E1A08B204742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -789,26 +789,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" customWidth="1"/>
-    <col min="11" max="11" width="49.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="1"/>
+    <col min="11" max="11" width="49.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>86</v>
       </c>
@@ -843,7 +843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -857,7 +857,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>12</v>
@@ -878,7 +878,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -892,7 +892,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>17</v>
@@ -911,7 +911,7 @@
       </c>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -925,7 +925,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>21</v>
@@ -944,7 +944,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -977,7 +977,7 @@
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1208,7 +1208,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1740,7 +1740,7 @@
       </c>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1872,7 +1872,7 @@
       </c>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="K33" s="6"/>
     </row>
-    <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="K34" s="6"/>
     </row>
-    <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="K36" s="6"/>
     </row>
-    <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="K37" s="6"/>
     </row>
-    <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2072,7 +2072,7 @@
       </c>
       <c r="K38" s="6"/>
     </row>
-    <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
BT-B18-00-DUB-HLD-S2B0-01 dubleks buton listeye eklendi
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\Excel\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C318854-531D-4BB2-8548-BF21D468471A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5DCDB3-9FF6-4A43-BD5F-218328100464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="99">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>https://github.com/btk42/BT-B18-00-000-SLD-P3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-B18-00-DUB-HLD-S2B0-01</t>
   </si>
 </sst>
 </file>
@@ -792,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1477,7 +1480,9 @@
       <c r="J20" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K20" s="6"/>
+      <c r="K20" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
@@ -2156,9 +2161,10 @@
     <hyperlink ref="K14" r:id="rId5" xr:uid="{F83E4073-CF8D-4CCE-A9AD-3FC7038B5513}"/>
     <hyperlink ref="K35" r:id="rId6" xr:uid="{4DFC5FA9-97DC-48EE-B349-9B499628461D}"/>
     <hyperlink ref="K12" r:id="rId7" xr:uid="{7C1CE78A-8FC9-4F35-99E8-CA9B27D658BE}"/>
+    <hyperlink ref="K20" r:id="rId8" xr:uid="{CD2B8E64-7315-4F45-9FEC-9DE3067501C9}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Dubleks led kod hatası düzeltildi, 3lü konnektör eklendi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5DCDB3-9FF6-4A43-BD5F-218328100464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091C738B-3BF6-414B-ADDA-E40A9639FCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="100">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -171,9 +171,6 @@
     <t>3lü Konnektörlü</t>
   </si>
   <si>
-    <t>BT-B18-00-DUB-HLD-S2B0-01</t>
-  </si>
-  <si>
     <t>Dublex</t>
   </si>
   <si>
@@ -321,7 +318,13 @@
     <t>https://github.com/btk42/BT-B18-00-000-SLD-P3B1-01</t>
   </si>
   <si>
-    <t>https://github.com/btk42/BT-B18-00-DUB-HLD-S2B0-01</t>
+    <t>https://github.com/btk42/BT-B18-00-STP-SLD-P1B0-01</t>
+  </si>
+  <si>
+    <t>BT-B18-00-DUB-SLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-B18-00-DUB-SLD-S2B0-01</t>
   </si>
 </sst>
 </file>
@@ -795,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -816,7 +819,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -854,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
@@ -863,7 +866,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>12</v>
@@ -878,10 +881,10 @@
         <v>29</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -898,7 +901,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>17</v>
@@ -913,7 +916,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K3" s="6"/>
     </row>
@@ -931,7 +934,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>21</v>
@@ -946,7 +949,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K4" s="6"/>
     </row>
@@ -955,7 +958,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -979,7 +982,7 @@
         <v>29</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K5" s="6"/>
     </row>
@@ -1012,7 +1015,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -1045,7 +1048,7 @@
         <v>29</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -1078,7 +1081,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -1111,7 +1114,7 @@
         <v>29</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" s="6"/>
     </row>
@@ -1144,7 +1147,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="6"/>
     </row>
@@ -1153,7 +1156,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>34</v>
@@ -1177,7 +1180,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="6"/>
     </row>
@@ -1210,10 +1213,10 @@
         <v>29</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1245,7 +1248,7 @@
         <v>29</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" s="6"/>
     </row>
@@ -1278,10 +1281,10 @@
         <v>29</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1313,7 +1316,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K15" s="6"/>
     </row>
@@ -1346,7 +1349,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K16" s="6"/>
     </row>
@@ -1379,7 +1382,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K17" s="6"/>
     </row>
@@ -1412,7 +1415,7 @@
         <v>19</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K18" s="6"/>
     </row>
@@ -1445,7 +1448,7 @@
         <v>19</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K19" s="6"/>
     </row>
@@ -1454,7 +1457,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>36</v>
@@ -1463,10 +1466,10 @@
         <v>11</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>22</v>
@@ -1478,10 +1481,10 @@
         <v>19</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1489,7 +1492,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>36</v>
@@ -1498,7 +1501,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>12</v>
@@ -1513,7 +1516,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K21" s="6"/>
     </row>
@@ -1522,7 +1525,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>36</v>
@@ -1531,7 +1534,7 @@
         <v>11</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>21</v>
@@ -1546,7 +1549,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -1555,7 +1558,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>36</v>
@@ -1564,7 +1567,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>12</v>
@@ -1579,7 +1582,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K23" s="6"/>
     </row>
@@ -1588,7 +1591,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>36</v>
@@ -1597,7 +1600,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>17</v>
@@ -1606,13 +1609,13 @@
         <v>13</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K24" s="6"/>
     </row>
@@ -1621,7 +1624,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>36</v>
@@ -1630,7 +1633,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>17</v>
@@ -1639,22 +1642,24 @@
         <v>13</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K25" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>36</v>
@@ -1663,7 +1668,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>17</v>
@@ -1672,16 +1677,16 @@
         <v>13</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1689,7 +1694,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>32</v>
@@ -1698,7 +1703,7 @@
         <v>11</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>12</v>
@@ -1713,7 +1718,7 @@
         <v>15</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K27" s="6"/>
     </row>
@@ -1722,7 +1727,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>32</v>
@@ -1731,7 +1736,7 @@
         <v>25</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>12</v>
@@ -1746,7 +1751,7 @@
         <v>15</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K28" s="6"/>
     </row>
@@ -1755,16 +1760,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="D29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>12</v>
@@ -1779,7 +1784,7 @@
         <v>15</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K29" s="6"/>
     </row>
@@ -1788,7 +1793,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>11</v>
@@ -1797,7 +1802,7 @@
         <v>11</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>21</v>
@@ -1812,7 +1817,7 @@
         <v>19</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K30" s="6"/>
     </row>
@@ -1821,7 +1826,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>43</v>
@@ -1830,7 +1835,7 @@
         <v>11</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>21</v>
@@ -1845,7 +1850,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K31" s="6"/>
     </row>
@@ -1854,7 +1859,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>43</v>
@@ -1863,7 +1868,7 @@
         <v>11</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>21</v>
@@ -1878,7 +1883,7 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K32" s="6"/>
     </row>
@@ -1887,16 +1892,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>21</v>
@@ -1911,7 +1916,7 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K33" s="6"/>
     </row>
@@ -1920,16 +1925,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>21</v>
@@ -1944,7 +1949,7 @@
         <v>19</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K34" s="6"/>
     </row>
@@ -1953,16 +1958,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="D35" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>21</v>
@@ -1977,10 +1982,10 @@
         <v>19</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1988,16 +1993,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>21</v>
@@ -2012,7 +2017,7 @@
         <v>19</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K36" s="6"/>
     </row>
@@ -2021,10 +2026,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>11</v>
@@ -2045,7 +2050,7 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K37" s="6"/>
     </row>
@@ -2054,16 +2059,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>12</v>
@@ -2078,7 +2083,7 @@
         <v>19</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K38" s="6"/>
     </row>
@@ -2087,7 +2092,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>36</v>
@@ -2096,7 +2101,7 @@
         <v>25</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>12</v>
@@ -2111,10 +2116,10 @@
         <v>15</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2122,10 +2127,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>25</v>
@@ -2146,10 +2151,10 @@
         <v>29</v>
       </c>
       <c r="J40" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K40" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2162,9 +2167,10 @@
     <hyperlink ref="K35" r:id="rId6" xr:uid="{4DFC5FA9-97DC-48EE-B349-9B499628461D}"/>
     <hyperlink ref="K12" r:id="rId7" xr:uid="{7C1CE78A-8FC9-4F35-99E8-CA9B27D658BE}"/>
     <hyperlink ref="K20" r:id="rId8" xr:uid="{CD2B8E64-7315-4F45-9FEC-9DE3067501C9}"/>
+    <hyperlink ref="K25" r:id="rId9" xr:uid="{40681036-EED8-47DD-8C6A-9E141C5B164F}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
sub Buton Özelliği eklendi
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BTK\Ürün_Listesi\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A20D10-9E50-42B5-8BAF-E57D6D74CA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC746E2-31C8-4091-8B76-C86D963BE515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="112">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>BT-SQR-00-000-SLD-H3B0-02</t>
+  </si>
+  <si>
+    <t>BT-PNT-00-SUB-HLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>Sub Buton</t>
   </si>
 </sst>
 </file>
@@ -448,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -478,6 +484,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -829,28 +838,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" customWidth="1"/>
-    <col min="11" max="11" width="49.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="1"/>
+    <col min="11" max="11" width="49.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>85</v>
       </c>
@@ -885,7 +894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -920,7 +929,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -953,7 +962,7 @@
       </c>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -986,7 +995,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1019,7 +1028,7 @@
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1052,7 +1061,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1085,7 +1094,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1118,7 +1127,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1153,7 +1162,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1188,7 +1197,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1221,7 +1230,7 @@
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1254,7 +1263,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1287,7 +1296,7 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1322,7 +1331,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1355,7 +1364,7 @@
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1388,7 +1397,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1421,7 +1430,7 @@
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1454,7 +1463,7 @@
       </c>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1489,7 +1498,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1524,7 +1533,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1557,7 +1566,7 @@
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1590,7 +1599,7 @@
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1623,7 +1632,7 @@
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1656,7 +1665,7 @@
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1691,7 +1700,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1726,7 +1735,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1761,7 +1770,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1796,7 +1805,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1831,7 +1840,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1866,7 +1875,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1899,7 +1908,7 @@
       </c>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1932,7 +1941,7 @@
       </c>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1965,7 +1974,7 @@
       </c>
       <c r="K33" s="6"/>
     </row>
-    <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1998,7 +2007,7 @@
       </c>
       <c r="K34" s="6"/>
     </row>
-    <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2033,7 +2042,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2066,7 +2075,7 @@
       </c>
       <c r="K36" s="6"/>
     </row>
-    <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2099,7 +2108,7 @@
       </c>
       <c r="K37" s="6"/>
     </row>
-    <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2132,7 +2141,7 @@
       </c>
       <c r="K38" s="6"/>
     </row>
-    <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2167,7 +2176,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -2202,11 +2211,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="11" t="s">
         <v>109</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -2235,6 +2244,38 @@
       </c>
       <c r="K41" s="7" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="11">
+        <v>41</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Penta sub buton Eklendi
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BTK\Ürün_Listesi\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC746E2-31C8-4091-8B76-C86D963BE515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031A3025-C4C7-4521-AE63-A8550CC3333D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="111">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -238,9 +238,6 @@
   </si>
   <si>
     <t>BT-PNT-00-7BT-DLD-S2B0-01</t>
-  </si>
-  <si>
-    <t>BT-PNT-00-4BT-DLD-S2B0-01</t>
   </si>
   <si>
     <t>BT-EKA-00-7BT-DLD-S2B0-01</t>
@@ -838,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -861,7 +858,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -899,7 +896,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
@@ -923,10 +920,10 @@
         <v>29</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -958,7 +955,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K3" s="6"/>
     </row>
@@ -991,7 +988,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K4" s="6"/>
     </row>
@@ -1000,7 +997,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -1024,7 +1021,7 @@
         <v>29</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K5" s="6"/>
     </row>
@@ -1057,7 +1054,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -1090,7 +1087,7 @@
         <v>29</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -1123,7 +1120,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -1156,10 +1153,10 @@
         <v>29</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1191,10 +1188,10 @@
         <v>19</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1202,7 +1199,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>34</v>
@@ -1226,7 +1223,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K11" s="6"/>
     </row>
@@ -1259,7 +1256,7 @@
         <v>29</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K12" s="6"/>
     </row>
@@ -1292,7 +1289,7 @@
         <v>29</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K13" s="6"/>
     </row>
@@ -1325,10 +1322,10 @@
         <v>29</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1360,7 +1357,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K15" s="6"/>
     </row>
@@ -1393,7 +1390,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K16" s="6"/>
     </row>
@@ -1426,7 +1423,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K17" s="6"/>
     </row>
@@ -1459,7 +1456,7 @@
         <v>19</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K18" s="6"/>
     </row>
@@ -1492,10 +1489,10 @@
         <v>19</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1512,7 +1509,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>17</v>
@@ -1527,10 +1524,10 @@
         <v>19</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1562,7 +1559,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K21" s="6"/>
     </row>
@@ -1595,7 +1592,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -1628,7 +1625,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K23" s="6"/>
     </row>
@@ -1646,7 +1643,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>17</v>
@@ -1661,7 +1658,7 @@
         <v>19</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K24" s="6"/>
     </row>
@@ -1694,10 +1691,10 @@
         <v>19</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1729,10 +1726,10 @@
         <v>19</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1764,10 +1761,10 @@
         <v>15</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1799,10 +1796,10 @@
         <v>15</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1834,10 +1831,10 @@
         <v>15</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1845,7 +1842,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>11</v>
@@ -1854,7 +1851,7 @@
         <v>11</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>21</v>
@@ -1869,10 +1866,10 @@
         <v>19</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1904,7 +1901,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K31" s="6"/>
     </row>
@@ -1937,7 +1934,7 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K32" s="6"/>
     </row>
@@ -1970,7 +1967,7 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K33" s="6"/>
     </row>
@@ -1982,13 +1979,13 @@
         <v>71</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>21</v>
@@ -2003,25 +2000,27 @@
         <v>19</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K34" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="D35" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>21</v>
@@ -2036,11 +2035,9 @@
         <v>19</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K35" s="7" t="s">
-        <v>95</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="K35" s="6"/>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -2050,13 +2047,13 @@
         <v>74</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>21</v>
@@ -2071,7 +2068,7 @@
         <v>19</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K36" s="6"/>
     </row>
@@ -2080,19 +2077,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="D37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>22</v>
@@ -2104,7 +2101,7 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K37" s="6"/>
     </row>
@@ -2113,81 +2110,83 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K38" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="A39" s="9">
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K39" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>87</v>
+      <c r="B40" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>11</v>
@@ -2196,102 +2195,67 @@
         <v>17</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+        <v>101</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="11">
         <v>40</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G41" s="5" t="s">
+      <c r="C41" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="K41" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11">
-        <v>41</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H42" s="11" t="s">
+      <c r="H41" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" s="11" t="s">
-        <v>82</v>
+      <c r="I41" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" xr:uid="{4D1368D8-93A2-4595-A7F7-561AA1E0B8EC}"/>
-    <hyperlink ref="K39" r:id="rId2" xr:uid="{C18926DB-EDF7-459C-921F-7CF9DECA75BD}"/>
+    <hyperlink ref="K38" r:id="rId2" xr:uid="{C18926DB-EDF7-459C-921F-7CF9DECA75BD}"/>
     <hyperlink ref="K26" r:id="rId3" xr:uid="{4BB1A615-20FE-40BE-9BCA-4E34F0B63682}"/>
     <hyperlink ref="K14" r:id="rId4" xr:uid="{CB474D2C-5626-407C-A469-2AF2796A842F}"/>
-    <hyperlink ref="K35" r:id="rId5" xr:uid="{9FDBCB92-A2F0-4180-9A0F-F75D7F08C300}"/>
+    <hyperlink ref="K34" r:id="rId5" xr:uid="{9FDBCB92-A2F0-4180-9A0F-F75D7F08C300}"/>
     <hyperlink ref="K19" r:id="rId6" xr:uid="{6A31EF04-7D9C-47AA-980F-1628C2CAFCD2}"/>
     <hyperlink ref="K20" r:id="rId7" xr:uid="{C0C3334D-06DE-4FC7-9242-5B224D073786}"/>
     <hyperlink ref="K25" r:id="rId8" xr:uid="{71D038FE-AF8F-4144-992E-17A293F68C5A}"/>
     <hyperlink ref="K30" r:id="rId9" xr:uid="{E233DE4F-1AF6-4850-A43A-6B428181756A}"/>
     <hyperlink ref="K29" r:id="rId10" xr:uid="{F4B634F3-50EE-4BBC-9EE5-7575A10F5FA7}"/>
-    <hyperlink ref="K40" r:id="rId11" xr:uid="{EA6829D2-93ED-4D44-8854-9DAED99F0BCC}"/>
-    <hyperlink ref="K41" r:id="rId12" xr:uid="{E59630A8-B1EA-44C9-90E8-E1D739438F33}"/>
+    <hyperlink ref="K39" r:id="rId11" xr:uid="{EA6829D2-93ED-4D44-8854-9DAED99F0BCC}"/>
+    <hyperlink ref="K40" r:id="rId12" xr:uid="{E59630A8-B1EA-44C9-90E8-E1D739438F33}"/>
     <hyperlink ref="K9" r:id="rId13" xr:uid="{860E6201-CDD5-4E0D-B258-B022CC8CF354}"/>
     <hyperlink ref="K10" r:id="rId14" xr:uid="{86414EDF-DE52-4FB4-941A-B0E6970EE722}"/>
     <hyperlink ref="K27" r:id="rId15" xr:uid="{F775A0C6-E437-46E3-B551-2C2849DDDF2A}"/>

</xml_diff>

<commit_message>
MSW buton,kod ve donanım eklendi
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BTK\Ürün_Listesi\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031A3025-C4C7-4521-AE63-A8550CC3333D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15414E83-9750-45BC-AD3F-1B5F2B1FE226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="114">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -357,7 +357,16 @@
     <t>BT-PNT-00-SUB-HLD-S2B0-01</t>
   </si>
   <si>
-    <t>Sub Buton</t>
+    <t>Sub Tümleşik Buton</t>
+  </si>
+  <si>
+    <t>MSW</t>
+  </si>
+  <si>
+    <t>BT-MSW-00-00-SLD-H3B0-03</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-MSW-00-00-SLD-H3B0-03</t>
   </si>
 </sst>
 </file>
@@ -835,28 +844,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" style="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" customWidth="1"/>
-    <col min="11" max="11" width="49.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.5703125" style="1"/>
+    <col min="11" max="11" width="49.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>84</v>
       </c>
@@ -891,7 +900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -926,7 +935,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -959,7 +968,7 @@
       </c>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -992,7 +1001,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1025,7 +1034,7 @@
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1058,7 +1067,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1091,7 +1100,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1124,7 +1133,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1159,7 +1168,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1194,7 +1203,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1227,7 +1236,7 @@
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1260,7 +1269,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1293,7 +1302,7 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1328,7 +1337,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1361,7 +1370,7 @@
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1394,7 +1403,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1427,7 +1436,7 @@
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1460,7 +1469,7 @@
       </c>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1495,7 +1504,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1530,7 +1539,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1563,7 +1572,7 @@
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1596,7 +1605,7 @@
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1629,7 +1638,7 @@
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1662,7 +1671,7 @@
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1697,7 +1706,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1732,7 +1741,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1767,7 +1776,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1802,7 +1811,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1837,7 +1846,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1872,7 +1881,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1905,7 +1914,7 @@
       </c>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1919,7 +1928,7 @@
         <v>11</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>21</v>
@@ -1938,7 +1947,7 @@
       </c>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1971,7 +1980,7 @@
       </c>
       <c r="K33" s="6"/>
     </row>
-    <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2006,7 +2015,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2039,7 +2048,7 @@
       </c>
       <c r="K35" s="6"/>
     </row>
-    <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2072,7 +2081,7 @@
       </c>
       <c r="K36" s="6"/>
     </row>
-    <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2105,7 +2114,7 @@
       </c>
       <c r="K37" s="6"/>
     </row>
-    <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2140,7 +2149,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -2175,7 +2184,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2210,7 +2219,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>40</v>
       </c>
@@ -2240,6 +2249,41 @@
       </c>
       <c r="J41" s="11" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11">
+        <v>40</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2260,9 +2304,10 @@
     <hyperlink ref="K10" r:id="rId14" xr:uid="{86414EDF-DE52-4FB4-941A-B0E6970EE722}"/>
     <hyperlink ref="K27" r:id="rId15" xr:uid="{F775A0C6-E437-46E3-B551-2C2849DDDF2A}"/>
     <hyperlink ref="K28" r:id="rId16" xr:uid="{5E424020-A8AB-429D-BA19-B25C10F99E29}"/>
+    <hyperlink ref="K42" r:id="rId17" xr:uid="{31BDDBC5-37DF-4659-A3E3-403FB87620B6}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId18"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Bir kaç buton eklenmiştir
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983679AA-5E71-4A17-BECF-C221BA61A75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3E3894-2F40-47D1-A01B-57366B6DEA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="125">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -180,9 +180,6 @@
     <t>BT-B18-00-2SW-DLD-S3B0-01</t>
   </si>
   <si>
-    <t>BT-B18-00-MSC-HLD-S2B0-01</t>
-  </si>
-  <si>
     <t>Mikel Dual</t>
   </si>
   <si>
@@ -394,6 +391,15 @@
   </si>
   <si>
     <t>https://github.com/btk42/BT-ANV-00-000-SLD-H3B0-01</t>
+  </si>
+  <si>
+    <t>BT-B18-00-MSC-HLD-S2B2-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-B18-00-MSC-HLD-S2B2-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-B18-00-000-DLD-S2B0-01</t>
   </si>
 </sst>
 </file>
@@ -874,7 +880,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -894,7 +900,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -932,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
@@ -956,10 +962,10 @@
         <v>29</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -991,10 +997,10 @@
         <v>19</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1026,7 +1032,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K4" s="6"/>
     </row>
@@ -1035,7 +1041,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -1059,7 +1065,7 @@
         <v>29</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K5" s="6"/>
     </row>
@@ -1092,7 +1098,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -1125,7 +1131,7 @@
         <v>29</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -1158,7 +1164,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -1167,7 +1173,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>31</v>
@@ -1191,10 +1197,10 @@
         <v>29</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1226,10 +1232,10 @@
         <v>19</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1237,7 +1243,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>33</v>
@@ -1261,7 +1267,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K11" s="6"/>
     </row>
@@ -1294,7 +1300,7 @@
         <v>29</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K12" s="6"/>
     </row>
@@ -1327,7 +1333,7 @@
         <v>29</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K13" s="6"/>
     </row>
@@ -1360,10 +1366,10 @@
         <v>29</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1395,7 +1401,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K15" s="6"/>
     </row>
@@ -1428,7 +1434,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K16" s="6"/>
     </row>
@@ -1461,7 +1467,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K17" s="6"/>
     </row>
@@ -1494,9 +1500,11 @@
         <v>19</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="K18" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
@@ -1527,10 +1535,10 @@
         <v>19</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1547,7 +1555,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>17</v>
@@ -1562,10 +1570,10 @@
         <v>19</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1597,7 +1605,7 @@
         <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K21" s="6"/>
     </row>
@@ -1630,7 +1638,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -1639,7 +1647,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>51</v>
+        <v>122</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>35</v>
@@ -1648,7 +1656,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>12</v>
@@ -1660,19 +1668,21 @@
         <v>23</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="K23" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>35</v>
@@ -1681,7 +1691,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>17</v>
@@ -1690,13 +1700,13 @@
         <v>13</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K24" s="6"/>
     </row>
@@ -1705,7 +1715,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>35</v>
@@ -1714,7 +1724,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>17</v>
@@ -1723,16 +1733,16 @@
         <v>13</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1740,7 +1750,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>35</v>
@@ -1749,7 +1759,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>17</v>
@@ -1758,16 +1768,16 @@
         <v>13</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1775,7 +1785,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>31</v>
@@ -1784,7 +1794,7 @@
         <v>11</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>12</v>
@@ -1799,10 +1809,10 @@
         <v>15</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1810,7 +1820,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>31</v>
@@ -1819,7 +1829,7 @@
         <v>25</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>12</v>
@@ -1834,10 +1844,10 @@
         <v>15</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1845,16 +1855,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="D29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>12</v>
@@ -1869,10 +1879,10 @@
         <v>15</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1880,7 +1890,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>11</v>
@@ -1889,7 +1899,7 @@
         <v>11</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>21</v>
@@ -1904,10 +1914,10 @@
         <v>19</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1915,7 +1925,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>42</v>
@@ -1924,7 +1934,7 @@
         <v>11</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>21</v>
@@ -1939,7 +1949,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K31" s="6"/>
     </row>
@@ -1948,7 +1958,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>42</v>
@@ -1957,7 +1967,7 @@
         <v>11</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>21</v>
@@ -1972,7 +1982,7 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K32" s="6"/>
     </row>
@@ -1981,16 +1991,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>21</v>
@@ -2005,7 +2015,7 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K33" s="6"/>
     </row>
@@ -2014,16 +2024,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="D34" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>21</v>
@@ -2038,10 +2048,10 @@
         <v>19</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2049,16 +2059,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>21</v>
@@ -2073,7 +2083,7 @@
         <v>19</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K35" s="6"/>
     </row>
@@ -2082,10 +2092,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>11</v>
@@ -2106,7 +2116,7 @@
         <v>19</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K36" s="6"/>
     </row>
@@ -2115,16 +2125,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>12</v>
@@ -2139,7 +2149,7 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K37" s="6"/>
     </row>
@@ -2148,7 +2158,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>35</v>
@@ -2157,7 +2167,7 @@
         <v>25</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>12</v>
@@ -2172,10 +2182,10 @@
         <v>15</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2183,10 +2193,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>25</v>
@@ -2207,10 +2217,10 @@
         <v>29</v>
       </c>
       <c r="J39" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K39" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2218,10 +2228,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>11</v>
@@ -2242,10 +2252,10 @@
         <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2253,16 +2263,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>12</v>
@@ -2277,7 +2287,7 @@
         <v>19</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2285,10 +2295,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>11</v>
@@ -2309,10 +2319,10 @@
         <v>19</v>
       </c>
       <c r="J42" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2320,10 +2330,10 @@
         <v>43</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>11</v>
@@ -2344,10 +2354,10 @@
         <v>19</v>
       </c>
       <c r="J43" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2355,10 +2365,10 @@
         <v>44</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>11</v>
@@ -2379,10 +2389,10 @@
         <v>29</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2390,10 +2400,10 @@
         <v>45</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>11</v>
@@ -2414,10 +2424,10 @@
         <v>19</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2443,9 +2453,11 @@
     <hyperlink ref="K44" r:id="rId19" xr:uid="{374D957E-1A4B-49F5-B459-E485D998364A}"/>
     <hyperlink ref="K45" r:id="rId20" xr:uid="{C60D8AE6-2975-4887-B335-13A8689090EF}"/>
     <hyperlink ref="K3" r:id="rId21" xr:uid="{0B81BF3F-699C-42BF-A1AC-8D5E46DE2666}"/>
+    <hyperlink ref="K23" r:id="rId22" xr:uid="{BC3D4A1D-7BEA-42FA-87EA-BF5C561DF9B2}"/>
+    <hyperlink ref="K18" r:id="rId23" xr:uid="{E95298E8-A877-40E0-988B-62B5F3BA442B}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId24"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
listedekiler %100 kalktı, liste dışı ekleniyor
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570D4720-2BC7-4C05-96CE-98D5D512D63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA409F8-5B40-46A5-986B-C841F18371F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="156">
   <si>
     <t>Ürün Kodu</t>
   </si>
@@ -213,24 +213,12 @@
     <t>7li Tümleşik Buton</t>
   </si>
   <si>
-    <t>BT-NVA-00-4BT-DLD-S2B0-01</t>
-  </si>
-  <si>
-    <t>4lü Tümleşik Buton</t>
-  </si>
-  <si>
     <t>BT-PNT-00-7BT-DLD-S2B0-01</t>
   </si>
   <si>
-    <t>BT-EKA-00-7BT-DLD-S2B0-01</t>
-  </si>
-  <si>
     <t>Eka</t>
   </si>
   <si>
-    <t>BT-EKA-00-4BT-DLD-S2B0-01</t>
-  </si>
-  <si>
     <t>BT-PRL-00-000-DLD-S2B0-01</t>
   </si>
   <si>
@@ -282,9 +270,6 @@
     <t>https://github.com/btk42/BT-B18-OS-000-HLD-P3B1-01</t>
   </si>
   <si>
-    <t>https://github.com/btk42/BT-EKA-00-7BT-DLD-S2B0-01</t>
-  </si>
-  <si>
     <t>https://github.com/btk42/BT-B18-00-3CN-SLD-S2B0-01</t>
   </si>
   <si>
@@ -330,9 +315,6 @@
     <t>BT-PNT-00-SUB-HLD-S2B0-01</t>
   </si>
   <si>
-    <t>Sub Tümleşik Buton</t>
-  </si>
-  <si>
     <t>MSW</t>
   </si>
   <si>
@@ -460,6 +442,57 @@
   </si>
   <si>
     <t>BT-B18-00-TKI-SLD-P3B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-PRL-00-000-DLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-PRL-00-MSC-DLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-NVA-00-000-HLD-H2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-NVA-00-7BT-DLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-PNT-00-7BT-DLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>Alt Tümleşik Buton</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-PNT-00-SUB-HLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>BT-NVA-00-SUB-DLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>BT-EKA-00-SUB-DLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-NVA-00-SUB-DLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-EKA-00-SUB-DLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>BT-EKA-00-7BT-DLD-S2B0-02</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-EKA-00-7BT-DLD-S2B0-02</t>
+  </si>
+  <si>
+    <t>BT-PNT-00-000-SLD-H2B0-01</t>
+  </si>
+  <si>
+    <t>BT-PNT-00-000-SLD-H2B0-02</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-PNT-00-000-SLD-H2B0-02</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-PNT-00-000-SLD-H2B0-01</t>
   </si>
 </sst>
 </file>
@@ -553,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -569,9 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -937,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -960,7 +990,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -998,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
@@ -1022,10 +1052,10 @@
         <v>29</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>141</v>
+        <v>87</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1057,10 +1087,10 @@
         <v>19</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>113</v>
+        <v>70</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1092,10 +1122,10 @@
         <v>19</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>113</v>
+        <v>70</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1103,7 +1133,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>24</v>
@@ -1127,10 +1157,10 @@
         <v>29</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>139</v>
+        <v>70</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1162,10 +1192,10 @@
         <v>19</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>132</v>
+        <v>70</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1197,10 +1227,10 @@
         <v>29</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>133</v>
+        <v>70</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1232,10 +1262,10 @@
         <v>19</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>127</v>
+        <v>70</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1243,7 +1273,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>31</v>
@@ -1267,10 +1297,10 @@
         <v>29</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>95</v>
+        <v>70</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1302,10 +1332,10 @@
         <v>19</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>96</v>
+        <v>70</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1313,7 +1343,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>33</v>
@@ -1337,10 +1367,10 @@
         <v>29</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>128</v>
+        <v>70</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1372,10 +1402,10 @@
         <v>29</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>121</v>
+        <v>70</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1383,7 +1413,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>35</v>
@@ -1407,10 +1437,10 @@
         <v>29</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>137</v>
+        <v>70</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1442,10 +1472,10 @@
         <v>29</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>84</v>
+        <v>70</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1453,7 +1483,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>35</v>
@@ -1477,10 +1507,10 @@
         <v>19</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>123</v>
+        <v>70</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1503,7 +1533,7 @@
         <v>12</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>23</v>
@@ -1512,16 +1542,18 @@
         <v>19</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K16" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>35</v>
@@ -1545,10 +1577,10 @@
         <v>19</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>135</v>
+        <v>70</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1580,10 +1612,10 @@
         <v>19</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>116</v>
+        <v>70</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1615,10 +1647,10 @@
         <v>19</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>86</v>
+        <v>70</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1635,7 +1667,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>17</v>
@@ -1650,10 +1682,10 @@
         <v>19</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>91</v>
+        <v>70</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1661,7 +1693,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>35</v>
@@ -1685,10 +1717,10 @@
         <v>19</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>125</v>
+        <v>70</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1720,10 +1752,10 @@
         <v>19</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>126</v>
+        <v>70</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1731,7 +1763,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>35</v>
@@ -1755,10 +1787,10 @@
         <v>15</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>115</v>
+        <v>70</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1775,7 +1807,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>17</v>
@@ -1790,10 +1822,10 @@
         <v>19</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>120</v>
+        <v>70</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1825,10 +1857,10 @@
         <v>19</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>87</v>
+        <v>70</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1860,10 +1892,10 @@
         <v>19</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>83</v>
+        <v>70</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1895,10 +1927,10 @@
         <v>15</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>97</v>
+        <v>70</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1930,10 +1962,10 @@
         <v>15</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1965,10 +1997,10 @@
         <v>15</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>88</v>
+        <v>70</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1976,7 +2008,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>11</v>
@@ -1985,7 +2017,7 @@
         <v>11</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>21</v>
@@ -2000,10 +2032,10 @@
         <v>19</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2035,16 +2067,18 @@
         <v>19</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K31" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>40</v>
@@ -2052,8 +2086,8 @@
       <c r="D32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>101</v>
+      <c r="E32" s="10" t="s">
+        <v>144</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>21</v>
@@ -2068,16 +2102,18 @@
         <v>19</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K32" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>58</v>
@@ -2101,19 +2137,21 @@
         <v>19</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K33" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="34" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>11</v>
@@ -2134,10 +2172,10 @@
         <v>19</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>85</v>
+        <v>70</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2145,16 +2183,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>67</v>
+        <v>147</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>63</v>
+      <c r="E35" s="10" t="s">
+        <v>144</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>21</v>
@@ -2169,19 +2207,21 @@
         <v>19</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K35" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>11</v>
@@ -2202,19 +2242,21 @@
         <v>19</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K36" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>11</v>
@@ -2223,7 +2265,7 @@
         <v>47</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>22</v>
@@ -2235,16 +2277,18 @@
         <v>19</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K37" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="38" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>35</v>
@@ -2253,7 +2297,7 @@
         <v>25</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>12</v>
@@ -2268,21 +2312,21 @@
         <v>15</v>
       </c>
       <c r="J38" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="K38" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>25</v>
@@ -2303,21 +2347,21 @@
         <v>29</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>99</v>
+      <c r="B40" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>11</v>
@@ -2338,58 +2382,61 @@
         <v>19</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11">
+        <v>87</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
         <v>40</v>
       </c>
-      <c r="B41" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C41" s="11" t="s">
+      <c r="B41" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F41" s="11" t="s">
+      <c r="D41" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G41" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="11" t="s">
+      <c r="H41" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I41" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" s="11" t="s">
-        <v>74</v>
+      <c r="I41" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11">
+      <c r="A42" s="10">
         <v>41</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="11" t="s">
+      <c r="B42" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F42" s="5" t="s">
@@ -2401,30 +2448,30 @@
       <c r="H42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I42" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>104</v>
+      <c r="I42" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="11" t="s">
+      <c r="B43" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F43" s="5" t="s">
@@ -2436,14 +2483,14 @@
       <c r="H43" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I43" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J43" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="K43" s="7" t="s">
-        <v>106</v>
+      <c r="I43" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2451,10 +2498,10 @@
         <v>44</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>11</v>
@@ -2475,10 +2522,10 @@
         <v>29</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>111</v>
+        <v>70</v>
+      </c>
+      <c r="K44" s="9" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2486,10 +2533,10 @@
         <v>45</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>11</v>
@@ -2510,26 +2557,26 @@
         <v>19</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K45" s="10" t="s">
-        <v>112</v>
+        <v>70</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>46</v>
       </c>
-      <c r="B46" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="11" t="s">
+      <c r="B46" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F46" s="5" t="s">
@@ -2544,11 +2591,11 @@
       <c r="I46" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J46" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="K46" s="7" t="s">
-        <v>119</v>
+      <c r="J46" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2556,7 +2603,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>35</v>
@@ -2565,7 +2612,7 @@
         <v>11</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>12</v>
@@ -2580,10 +2627,10 @@
         <v>15</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K47" s="7" t="s">
-        <v>131</v>
+        <v>70</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2591,7 +2638,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>35</v>
@@ -2600,7 +2647,7 @@
         <v>11</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>17</v>
@@ -2615,10 +2662,80 @@
         <v>29</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K48" s="10" t="s">
-        <v>143</v>
+        <v>70</v>
+      </c>
+      <c r="K48" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>49</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>50</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2662,9 +2779,19 @@
     <hyperlink ref="K5" r:id="rId37" xr:uid="{5EB2195E-491D-4564-A007-401534844A2D}"/>
     <hyperlink ref="K11" r:id="rId38" xr:uid="{D2DA8399-A694-4C03-B894-94FCB46C1C82}"/>
     <hyperlink ref="K48" r:id="rId39" xr:uid="{8BEDF4AB-715B-4834-96A1-3B238E40A55A}"/>
+    <hyperlink ref="K36" r:id="rId40" xr:uid="{45C4C12C-53D7-41C9-93FC-BBF4F2C385CF}"/>
+    <hyperlink ref="K37" r:id="rId41" xr:uid="{E7B30BE2-EAED-46B0-9FE3-30CF00FE8ED3}"/>
+    <hyperlink ref="K16" r:id="rId42" xr:uid="{5CA4000B-8FB8-4D08-8058-92063D0BB344}"/>
+    <hyperlink ref="K41" r:id="rId43" xr:uid="{18813AFE-BC32-4574-AE07-C8E9379F2D22}"/>
+    <hyperlink ref="K31" r:id="rId44" xr:uid="{B1596BB4-522A-4B72-B2B3-0F4F660EC1E2}"/>
+    <hyperlink ref="K32" r:id="rId45" xr:uid="{AEEA70CB-9DDD-4E7B-82D2-02208B9265ED}"/>
+    <hyperlink ref="K33" r:id="rId46" xr:uid="{0511C719-7AB2-4ED3-B1A3-E801B77588C3}"/>
+    <hyperlink ref="K35" r:id="rId47" xr:uid="{C7177745-5FF6-48B3-A3E6-AECEE74E6216}"/>
+    <hyperlink ref="K49" r:id="rId48" xr:uid="{95041AB1-B134-46DE-9FF3-60D891488450}"/>
+    <hyperlink ref="K50" r:id="rId49" xr:uid="{5DF6CBFE-9F41-45CE-BAA7-AF17D2584959}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId50"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>

<commit_message>
Eka 7 li tümleşik buton repo url uzantısı değiştirildi.
</commit_message>
<xml_diff>
--- a/pages/butonlar.xlsx
+++ b/pages/butonlar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Altium\GiTME\io_list\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA409F8-5B40-46A5-986B-C841F18371F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7097D496-BCDA-4BC9-B7BB-C10FB1673BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -477,12 +477,6 @@
     <t>https://github.com/btk42/BT-EKA-00-SUB-DLD-S2B0-01</t>
   </si>
   <si>
-    <t>BT-EKA-00-7BT-DLD-S2B0-02</t>
-  </si>
-  <si>
-    <t>https://github.com/btk42/BT-EKA-00-7BT-DLD-S2B0-02</t>
-  </si>
-  <si>
     <t>BT-PNT-00-000-SLD-H2B0-01</t>
   </si>
   <si>
@@ -493,6 +487,12 @@
   </si>
   <si>
     <t>https://github.com/btk42/BT-PNT-00-000-SLD-H2B0-01</t>
+  </si>
+  <si>
+    <t>BT-EKA-00-7BT-DLD-S2B0-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/BT-EKA-00-7BT-DLD-S2B0-01</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2148,7 +2148,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>63</v>
@@ -2175,7 +2175,7 @@
         <v>70</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2673,7 +2673,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>58</v>
@@ -2700,7 +2700,7 @@
         <v>70</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -2708,7 +2708,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>58</v>
@@ -2735,7 +2735,7 @@
         <v>87</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>